<commit_message>
MA0801: Actualización de seguimiento de producción digital
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_08_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_08_01_CO.xlsx
@@ -645,7 +645,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -721,8 +721,12 @@
       <c r="E4" s="15">
         <v>42087.773611111108</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="F4" s="15">
+        <v>42088.680555555555</v>
+      </c>
+      <c r="G4" s="15">
+        <v>42089.68888883102</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>

</xml_diff>

<commit_message>
seguimiento grado 8 y 11
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_MA_08_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_MA_08_01_CO.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\seguimiento\ProduccionDigital\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21713" windowHeight="9711"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21720" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
   <si>
     <t>Cuaderno de estudio</t>
   </si>
@@ -198,6 +196,9 @@
   </si>
   <si>
     <t>SÍ</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -277,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +309,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -319,29 +332,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -349,23 +362,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -373,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -399,9 +412,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -411,6 +421,18 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -420,16 +442,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,7 +517,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,7 +552,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -704,7 +729,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -714,39 +739,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5:C24"/>
+      <selection pane="topRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="47.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="12.06640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.100000000000001" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G2" s="17" t="s">
+    <row r="2" spans="1:14">
+      <c r="G2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-    </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" ht="21.15" x14ac:dyDescent="0.45">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="22">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -765,19 +790,19 @@
       <c r="F3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -786,55 +811,63 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="15.85" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:14" ht="15">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="18">
         <v>42088.59375</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="18">
         <v>42089.688877314817</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="10" t="s">
+      <c r="G4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
+      <c r="C5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -843,42 +876,50 @@
       <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
+      <c r="D7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -887,42 +928,50 @@
       <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -931,42 +980,50 @@
       <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+      <c r="C11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="18"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -975,42 +1032,50 @@
       <c r="D12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="10" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="10" t="s">
+      <c r="C13" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1019,42 +1084,50 @@
       <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="18"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="10" t="s">
+      <c r="D15" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -1063,42 +1136,50 @@
       <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="10" t="s">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="18"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
+      <c r="D17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="18"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1107,42 +1188,50 @@
       <c r="D18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
+      <c r="C19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -1151,42 +1240,50 @@
       <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
+      <c r="D21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1195,42 +1292,50 @@
       <c r="D22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="15"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="10" t="s">
+      <c r="C23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="18"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -1239,14 +1344,18 @@
       <c r="D24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1258,6 +1367,11 @@
     <mergeCell ref="F4:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>